<commit_message>
ZSS-449 Freeze panels and change row/column size, then switch to other sheet and back, freeze panel's headers will be chaos.
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue/443-column-width.xlsx
+++ b/zss.test/src/main/webapp/issue/443-column-width.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zk\git\zkspreadsheet-2.x\zss.test\src\main\webapp\issue\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="16095" windowHeight="7710"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="16095" windowHeight="7710" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,9 +20,18 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>E8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +80,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -112,7 +134,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -144,9 +166,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -178,6 +201,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -353,15 +377,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -369,27 +393,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="8" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>